<commit_message>
app: working TP plots
</commit_message>
<xml_diff>
--- a/Part I/shiny app/par_to_hyp2.xlsx
+++ b/Part I/shiny app/par_to_hyp2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\Part I\shiny app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DE1686-D93D-4B22-9343-7C3B27E9E484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA823F91-1F42-41AC-8694-75861A25E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8304" yWindow="1272" windowWidth="9576" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8352" yWindow="3396" windowWidth="9576" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>n_par</t>
   </si>
@@ -124,13 +124,34 @@
   </si>
   <si>
     <t>$\beta_{1}&gt;\beta_{2} \hspace{0.3cm} \&amp; \hspace{0.3cm} \beta_{1}&gt;\beta_{3}$</t>
+  </si>
+  <si>
+    <t>dimname</t>
+  </si>
+  <si>
+    <t>H1.V1&gt;V2&gt;V3&gt;0</t>
+  </si>
+  <si>
+    <t>H1.complement</t>
+  </si>
+  <si>
+    <t>H2.V1&gt;V2&gt;V3</t>
+  </si>
+  <si>
+    <t>H2.complement</t>
+  </si>
+  <si>
+    <t>H3.V1&gt;V2&amp;0.6666667*V1&gt;V3</t>
+  </si>
+  <si>
+    <t>H3.complement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +164,12 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,9 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +492,7 @@
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +505,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -490,7 +523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -504,7 +537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -515,7 +548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -529,7 +562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -543,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -557,7 +590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -571,7 +604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -582,7 +615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -595,8 +628,11 @@
       <c r="D10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -609,8 +645,11 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -623,8 +662,11 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -637,8 +679,11 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -651,8 +696,11 @@
       <c r="D14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -665,8 +713,11 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -675,6 +726,9 @@
       </c>
       <c r="D16" t="s">
         <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempt to add 2 predictors
</commit_message>
<xml_diff>
--- a/Part I/shiny app/par_to_hyp2.xlsx
+++ b/Part I/shiny app/par_to_hyp2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\Part I\shiny app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA823F91-1F42-41AC-8694-75861A25E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D0C6C1-711B-44A5-A2EF-A5994F9CBDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8352" yWindow="3396" windowWidth="9576" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>n_par</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>H3.complement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1.V1&gt;V2&gt;0 </t>
+  </si>
+  <si>
+    <t>H2.V1&gt;V2</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +498,7 @@
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -523,7 +529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -537,7 +543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -548,7 +554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -561,8 +567,11 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -575,8 +584,11 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -589,8 +601,11 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -603,8 +618,11 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -614,8 +632,11 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -632,7 +653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -648,8 +669,9 @@
       <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -666,7 +688,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -683,7 +705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -700,7 +722,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -717,7 +739,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Revert "attempt to add 2 predictors"
This reverts commit e64a01d5e5f0cacf1e4c7c6059924bf3658c4e1d.
</commit_message>
<xml_diff>
--- a/Part I/shiny app/par_to_hyp2.xlsx
+++ b/Part I/shiny app/par_to_hyp2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\Part I\shiny app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D0C6C1-711B-44A5-A2EF-A5994F9CBDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA823F91-1F42-41AC-8694-75861A25E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8352" yWindow="3396" windowWidth="9576" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>n_par</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>H3.complement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1.V1&gt;V2&gt;0 </t>
-  </si>
-  <si>
-    <t>H2.V1&gt;V2</t>
   </si>
 </sst>
 </file>
@@ -486,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +492,7 @@
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,7 +523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -543,7 +537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -554,7 +548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -567,11 +561,8 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -584,11 +575,8 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -601,11 +589,8 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -618,11 +603,8 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -632,11 +614,8 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -653,7 +632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -669,9 +648,8 @@
       <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -688,7 +666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -705,7 +683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -722,7 +700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -739,7 +717,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>

</xml_diff>